<commit_message>
added day 2 data and code
</commit_message>
<xml_diff>
--- a/data/size/trial_size.xlsx
+++ b/data/size/trial_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/vims-resazurin/data/size/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1CF081-6F88-C54E-B1DE-7355BD4AF123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203091FD-C050-1F4E-AD20-21CBEF5DFE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="760" windowWidth="11960" windowHeight="17120" xr2:uid="{DD34C9EB-E2ED-8349-AB5F-FDE14F54E3E1}"/>
+    <workbookView xWindow="740" yWindow="760" windowWidth="11960" windowHeight="17120" xr2:uid="{DD34C9EB-E2ED-8349-AB5F-FDE14F54E3E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="48">
   <si>
     <t>date</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>plate12</t>
+  </si>
+  <si>
+    <t>plate15</t>
   </si>
 </sst>
 </file>
@@ -548,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAB0EB0-0DA4-F441-80F7-FBB69504C7E9}">
-  <dimension ref="A1:D461"/>
+  <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A449" workbookViewId="0">
+      <selection activeCell="G469" sqref="G469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7010,6 +7013,286 @@
         <v>16.77</v>
       </c>
     </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <v>20250701</v>
+      </c>
+      <c r="B462" t="s">
+        <v>47</v>
+      </c>
+      <c r="C462" t="s">
+        <v>4</v>
+      </c>
+      <c r="D462">
+        <v>16.59</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <v>20250701</v>
+      </c>
+      <c r="B463" t="s">
+        <v>47</v>
+      </c>
+      <c r="C463" t="s">
+        <v>5</v>
+      </c>
+      <c r="D463">
+        <v>14.06</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <v>20250701</v>
+      </c>
+      <c r="B464" t="s">
+        <v>47</v>
+      </c>
+      <c r="C464" t="s">
+        <v>6</v>
+      </c>
+      <c r="D464">
+        <v>13.44</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A465">
+        <v>20250701</v>
+      </c>
+      <c r="B465" t="s">
+        <v>47</v>
+      </c>
+      <c r="C465" t="s">
+        <v>7</v>
+      </c>
+      <c r="D465">
+        <v>14.97</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A466">
+        <v>20250701</v>
+      </c>
+      <c r="B466" t="s">
+        <v>47</v>
+      </c>
+      <c r="C466" t="s">
+        <v>8</v>
+      </c>
+      <c r="D466">
+        <v>16.36</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <v>20250701</v>
+      </c>
+      <c r="B467" t="s">
+        <v>47</v>
+      </c>
+      <c r="C467" t="s">
+        <v>9</v>
+      </c>
+      <c r="D467">
+        <v>15.82</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <v>20250701</v>
+      </c>
+      <c r="B468" t="s">
+        <v>47</v>
+      </c>
+      <c r="C468" t="s">
+        <v>10</v>
+      </c>
+      <c r="D468">
+        <v>12.16</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A469">
+        <v>20250701</v>
+      </c>
+      <c r="B469" t="s">
+        <v>47</v>
+      </c>
+      <c r="C469" t="s">
+        <v>11</v>
+      </c>
+      <c r="D469">
+        <v>14.12</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A470">
+        <v>20250701</v>
+      </c>
+      <c r="B470" t="s">
+        <v>47</v>
+      </c>
+      <c r="C470" t="s">
+        <v>12</v>
+      </c>
+      <c r="D470">
+        <v>13.39</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A471">
+        <v>20250701</v>
+      </c>
+      <c r="B471" t="s">
+        <v>47</v>
+      </c>
+      <c r="C471" t="s">
+        <v>13</v>
+      </c>
+      <c r="D471">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A472">
+        <v>20250701</v>
+      </c>
+      <c r="B472" t="s">
+        <v>47</v>
+      </c>
+      <c r="C472" t="s">
+        <v>14</v>
+      </c>
+      <c r="D472">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A473">
+        <v>20250701</v>
+      </c>
+      <c r="B473" t="s">
+        <v>47</v>
+      </c>
+      <c r="C473" t="s">
+        <v>15</v>
+      </c>
+      <c r="D473">
+        <v>14.49</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A474">
+        <v>20250701</v>
+      </c>
+      <c r="B474" t="s">
+        <v>47</v>
+      </c>
+      <c r="C474" t="s">
+        <v>16</v>
+      </c>
+      <c r="D474">
+        <v>14.98</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A475">
+        <v>20250701</v>
+      </c>
+      <c r="B475" t="s">
+        <v>47</v>
+      </c>
+      <c r="C475" t="s">
+        <v>17</v>
+      </c>
+      <c r="D475">
+        <v>14.72</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A476">
+        <v>20250701</v>
+      </c>
+      <c r="B476" t="s">
+        <v>47</v>
+      </c>
+      <c r="C476" t="s">
+        <v>18</v>
+      </c>
+      <c r="D476">
+        <v>13.38</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A477">
+        <v>20250701</v>
+      </c>
+      <c r="B477" t="s">
+        <v>47</v>
+      </c>
+      <c r="C477" t="s">
+        <v>19</v>
+      </c>
+      <c r="D477">
+        <v>13.68</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A478">
+        <v>20250701</v>
+      </c>
+      <c r="B478" t="s">
+        <v>47</v>
+      </c>
+      <c r="C478" t="s">
+        <v>20</v>
+      </c>
+      <c r="D478">
+        <v>16.63</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A479">
+        <v>20250701</v>
+      </c>
+      <c r="B479" t="s">
+        <v>47</v>
+      </c>
+      <c r="C479" t="s">
+        <v>21</v>
+      </c>
+      <c r="D479">
+        <v>12.58</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A480">
+        <v>20250701</v>
+      </c>
+      <c r="B480" t="s">
+        <v>47</v>
+      </c>
+      <c r="C480" t="s">
+        <v>22</v>
+      </c>
+      <c r="D480">
+        <v>13.47</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A481">
+        <v>20250701</v>
+      </c>
+      <c r="B481" t="s">
+        <v>47</v>
+      </c>
+      <c r="C481" t="s">
+        <v>23</v>
+      </c>
+      <c r="D481">
+        <v>13.81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added plate files and renamed files
</commit_message>
<xml_diff>
--- a/data/size/trial_size.xlsx
+++ b/data/size/trial_size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/vims-resazurin/data/size/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB05144F-A5CC-DC4E-B413-9404678F702B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF668FA9-3B5A-DA40-831C-2EDDF84A056A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="760" windowWidth="11960" windowHeight="17120" xr2:uid="{DD34C9EB-E2ED-8349-AB5F-FDE14F54E3E1}"/>
   </bookViews>
@@ -254,10 +254,10 @@
     <t>plate48</t>
   </si>
   <si>
-    <t>plateA</t>
+    <t>plate71</t>
   </si>
   <si>
-    <t>plateB</t>
+    <t>plate72</t>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAB0EB0-0DA4-F441-80F7-FBB69504C7E9}">
   <dimension ref="A1:D1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A468" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E484" sqref="E484"/>
+    <sheetView tabSelected="1" topLeftCell="A980" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C999" sqref="C999"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>